<commit_message>
train proximity to station code and csv
</commit_message>
<xml_diff>
--- a/datafiles_re_trains_stations/ptv_metro_train_station.xlsx
+++ b/datafiles_re_trains_stations/ptv_metro_train_station.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lglev_09wmwwo\Documents\Monash Uni working folder\Homework\Projects\Project1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lglev_09wmwwo\Documents\Monash Uni working folder\Homework\Project1\datafiles_re_trains_stations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA43FD8F-3A14-4B76-9E4B-B66BAA1F52BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97EE511-E73D-4B63-8CE8-4D2AB2C61AF8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ptv_metro_train_station" sheetId="1" r:id="rId1"/>
@@ -1471,7 +1471,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000000"/>
   </numFmts>
@@ -2310,7 +2310,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F222"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -2318,7 +2318,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="6.578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="60.578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="61" style="1" customWidth="1"/>
     <col min="3" max="4" width="19.578125" style="2" customWidth="1"/>
     <col min="5" max="5" width="10.578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="200.578125" style="1" customWidth="1"/>

</xml_diff>